<commit_message>
1) Consolidating PEM400 and EMM2816A into PRIME
</commit_message>
<xml_diff>
--- a/Hardware/LAB-ICM100/docs/LAB-ICM100-Rev0BOM.xlsx
+++ b/Hardware/LAB-ICM100/docs/LAB-ICM100-Rev0BOM.xlsx
@@ -298,15 +298,6 @@
   </si>
   <si>
     <t>Analog Devices</t>
-  </si>
-  <si>
-    <t>LAB-PEM300</t>
-  </si>
-  <si>
-    <t>LAB-PEM300ASSY</t>
-  </si>
-  <si>
-    <t>Board Assembly (LAB-PEM300)</t>
   </si>
   <si>
     <t>U1, U2</t>
@@ -430,6 +421,15 @@
   </si>
   <si>
     <t>10pc min, price is volatile</t>
+  </si>
+  <si>
+    <t>LAB-ICM100</t>
+  </si>
+  <si>
+    <t>LAB-ICM100ASSY</t>
+  </si>
+  <si>
+    <t>Board Assembly (LAB-ICM100)</t>
   </si>
 </sst>
 </file>
@@ -1401,7 +1401,7 @@
   <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,7 +1446,7 @@
         <v>80</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="3"/>
@@ -1460,7 +1460,7 @@
         <v>81</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="3"/>
@@ -1474,7 +1474,7 @@
         <v>82</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="D5" s="24"/>
       <c r="E5" s="3"/>
@@ -1529,10 +1529,10 @@
         <v>89</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>90</v>
@@ -1543,19 +1543,19 @@
         <v>1</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>93</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G9" s="16">
         <v>2</v>
@@ -1574,19 +1574,19 @@
         <v>2</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G10" s="16">
         <v>2</v>
@@ -1599,7 +1599,7 @@
         <v>0.79800000000000004</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1607,19 +1607,19 @@
         <v>3</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>92</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G11" s="16">
         <v>2</v>
@@ -1632,7 +1632,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1640,19 +1640,19 @@
         <v>4</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>92</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G12" s="16">
         <v>2</v>
@@ -1665,7 +1665,7 @@
         <v>0.63600000000000001</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1673,19 +1673,19 @@
         <v>5</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G13" s="16">
         <v>2</v>
@@ -1699,7 +1699,7 @@
         <v>0.2525</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1707,19 +1707,19 @@
         <v>6</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G14" s="16">
         <v>2</v>
@@ -1738,13 +1738,13 @@
         <v>7</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G15" s="12">
         <v>1</v>
@@ -1757,7 +1757,7 @@
         <v>10</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G16" s="12">
         <v>1</v>

</xml_diff>